<commit_message>
updates to 2 param
</commit_message>
<xml_diff>
--- a/book_data/Fitness.xlsx
+++ b/book_data/Fitness.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edmundlskoviak/Library/Mobile Documents/com~apple~CloudDocs/Data Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CC2697-2B48-494F-A486-C7F9A5AF60A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3639711-27B2-8344-B4DC-80F0D0736FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Non Walking" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -381,13 +381,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1014"/>
+  <dimension ref="A1:O1031"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O95" sqref="O95"/>
+      <selection pane="bottomRight" activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1805,1038 +1805,1412 @@
     </row>
     <row r="65" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>45600</v>
-      </c>
-      <c r="B65" s="2">
-        <v>179.2</v>
-      </c>
-      <c r="C65" s="2">
-        <v>24.9</v>
-      </c>
+        <v>45583</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
       <c r="D65" s="3">
-        <v>814</v>
-      </c>
-      <c r="E65" s="3">
-        <v>401</v>
+        <v>511</v>
+      </c>
+      <c r="E65" s="3"/>
+      <c r="I65" s="3">
+        <v>249</v>
       </c>
       <c r="M65" s="3">
-        <v>9071</v>
+        <v>11844</v>
       </c>
       <c r="N65">
-        <v>3.57</v>
+        <v>5</v>
       </c>
       <c r="O65">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>45601</v>
-      </c>
-      <c r="B66" s="2">
-        <v>180.2</v>
-      </c>
-      <c r="C66" s="2">
-        <v>24.9</v>
-      </c>
+        <v>45584</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
       <c r="D66" s="3">
-        <v>648</v>
-      </c>
-      <c r="F66" s="7">
-        <v>174</v>
+        <v>535</v>
+      </c>
+      <c r="E66" s="3"/>
+      <c r="I66" s="3">
+        <v>170</v>
       </c>
       <c r="M66" s="3">
-        <v>11332</v>
+        <v>1010</v>
       </c>
       <c r="N66">
-        <v>4.6500000000000004</v>
+        <v>425</v>
       </c>
       <c r="O66">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>45602</v>
-      </c>
-      <c r="B67" s="2">
-        <v>180.2</v>
-      </c>
-      <c r="C67" s="2">
-        <v>25.1</v>
-      </c>
+        <v>45585</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
       <c r="D67" s="3">
-        <v>995</v>
+        <v>813</v>
       </c>
       <c r="E67" s="3">
-        <v>366</v>
+        <v>359</v>
+      </c>
+      <c r="I67" s="3">
+        <v>117</v>
       </c>
       <c r="M67" s="3">
-        <v>12109</v>
+        <v>10953</v>
       </c>
       <c r="N67">
-        <v>4.8600000000000003</v>
+        <v>4.46</v>
       </c>
       <c r="O67">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>45603</v>
-      </c>
-      <c r="B68" s="2">
-        <v>179.7</v>
-      </c>
-      <c r="C68" s="2">
-        <v>24.9</v>
-      </c>
+        <v>45586</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
       <c r="D68" s="3">
-        <v>915</v>
+        <v>1026</v>
       </c>
       <c r="E68" s="3">
-        <v>384</v>
+        <v>388</v>
+      </c>
+      <c r="I68" s="3">
+        <v>252</v>
       </c>
       <c r="M68" s="3">
-        <v>12560</v>
+        <v>14872</v>
       </c>
       <c r="N68">
-        <v>5.0599999999999996</v>
+        <v>6.2</v>
       </c>
       <c r="O68">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>45605</v>
+        <v>45587</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="3">
-        <v>1089</v>
+        <v>794</v>
+      </c>
+      <c r="E69" s="3">
+        <v>350</v>
       </c>
       <c r="I69" s="3">
-        <v>297</v>
+        <v>82</v>
       </c>
       <c r="M69" s="3">
-        <v>22554</v>
+        <v>9189</v>
       </c>
       <c r="N69">
-        <v>8.86</v>
+        <v>3.7</v>
       </c>
       <c r="O69">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>45606</v>
+        <v>45588</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="3">
-        <v>1032</v>
-      </c>
-      <c r="E70" s="3">
-        <v>219</v>
-      </c>
+        <v>787</v>
+      </c>
+      <c r="E70" s="3"/>
       <c r="I70" s="3">
-        <v>88</v>
+        <v>443</v>
       </c>
       <c r="M70" s="3">
-        <v>16999</v>
-      </c>
-      <c r="N70" s="3">
-        <v>6.88</v>
-      </c>
-      <c r="O70" s="3">
-        <v>12</v>
+        <v>14942</v>
+      </c>
+      <c r="N70">
+        <v>6.57</v>
+      </c>
+      <c r="O70">
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>45607</v>
+        <v>45589</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3">
-        <v>1221</v>
-      </c>
-      <c r="F71" s="7">
-        <v>291</v>
-      </c>
-      <c r="L71" s="3">
-        <v>276</v>
-      </c>
+        <v>787</v>
+      </c>
+      <c r="E71" s="3">
+        <v>395</v>
+      </c>
+      <c r="I71" s="3"/>
       <c r="M71" s="3">
-        <v>15849</v>
-      </c>
-      <c r="N71" s="3">
-        <v>6.55</v>
-      </c>
-      <c r="O71" s="3">
-        <v>18</v>
+        <v>8070</v>
+      </c>
+      <c r="N71">
+        <v>3.22</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>45608</v>
+        <v>45590</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3">
-        <v>1147</v>
-      </c>
-      <c r="F72" s="7">
-        <v>193</v>
+        <v>871</v>
+      </c>
+      <c r="E72" s="3"/>
+      <c r="H72">
+        <v>228</v>
       </c>
       <c r="I72" s="3">
-        <v>131</v>
-      </c>
-      <c r="L72" s="3">
-        <v>218</v>
+        <v>116</v>
       </c>
       <c r="M72" s="3">
-        <v>16653</v>
-      </c>
-      <c r="N72" s="3">
-        <v>6.74</v>
-      </c>
-      <c r="O72" s="3">
-        <v>13</v>
+        <v>17697</v>
+      </c>
+      <c r="N72">
+        <v>7.52</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>45609</v>
+        <v>45591</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="3">
-        <v>1251</v>
-      </c>
-      <c r="F73" s="7">
-        <v>153</v>
-      </c>
-      <c r="I73" s="3">
-        <v>121</v>
-      </c>
-      <c r="L73" s="3">
-        <v>338</v>
-      </c>
+        <v>759</v>
+      </c>
+      <c r="E73" s="3">
+        <v>353</v>
+      </c>
+      <c r="I73" s="3"/>
       <c r="M73" s="3">
-        <v>16897</v>
-      </c>
-      <c r="N73" s="3">
-        <v>6.66</v>
-      </c>
-      <c r="O73" s="3">
-        <v>22</v>
+        <v>6536</v>
+      </c>
+      <c r="N73">
+        <v>2.59</v>
+      </c>
+      <c r="O73">
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>45610</v>
+        <v>45592</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="3">
-        <v>1033</v>
-      </c>
-      <c r="E74" s="3">
-        <v>250</v>
-      </c>
-      <c r="H74" s="3">
-        <v>118</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="E74" s="3"/>
+      <c r="I74" s="3"/>
       <c r="M74" s="3">
-        <v>14462</v>
-      </c>
-      <c r="N74" s="3">
-        <v>6.03</v>
-      </c>
-      <c r="O74" s="3">
-        <v>10</v>
+        <v>4772</v>
+      </c>
+      <c r="N74">
+        <v>1.89</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>45611</v>
+        <v>45593</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
       <c r="D75" s="3">
-        <v>882</v>
-      </c>
-      <c r="G75" s="3">
-        <v>227</v>
-      </c>
-      <c r="I75" s="3">
-        <v>36</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="E75" s="3"/>
+      <c r="I75" s="3"/>
       <c r="M75" s="3">
-        <v>12611</v>
-      </c>
-      <c r="N75" s="3">
-        <v>5.75</v>
-      </c>
-      <c r="O75" s="3">
-        <v>27</v>
+        <v>6720</v>
+      </c>
+      <c r="N75">
+        <v>2.66</v>
+      </c>
+      <c r="O75">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>45613</v>
+        <v>45594</v>
       </c>
       <c r="B76" s="2">
-        <v>180.6</v>
+        <v>179</v>
       </c>
       <c r="C76" s="2">
         <v>24.8</v>
       </c>
       <c r="D76" s="3">
-        <v>1146</v>
+        <v>892</v>
       </c>
       <c r="E76" s="3">
-        <v>439</v>
+        <v>339</v>
       </c>
       <c r="I76" s="3">
-        <v>207</v>
+        <v>110</v>
       </c>
       <c r="M76" s="3">
-        <v>16282</v>
-      </c>
-      <c r="N76" s="3">
-        <v>6.94</v>
-      </c>
-      <c r="O76" s="3">
-        <v>11</v>
+        <v>11739</v>
+      </c>
+      <c r="N76">
+        <v>4.72</v>
+      </c>
+      <c r="O76">
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>45614</v>
+        <v>45595</v>
       </c>
       <c r="B77" s="2">
-        <v>179.6</v>
+        <v>179</v>
       </c>
       <c r="C77" s="2">
-        <v>24.9</v>
+        <v>24.8</v>
       </c>
       <c r="D77" s="3">
-        <v>1057</v>
+        <v>1185</v>
       </c>
       <c r="E77" s="3">
-        <v>420</v>
+        <v>399</v>
+      </c>
+      <c r="H77">
+        <v>347</v>
       </c>
       <c r="I77" s="3">
-        <v>158</v>
+        <v>13</v>
       </c>
       <c r="M77" s="3">
-        <v>15864</v>
-      </c>
-      <c r="N77" s="3">
-        <v>6.53</v>
-      </c>
-      <c r="O77" s="3">
-        <v>4</v>
+        <v>14494</v>
+      </c>
+      <c r="N77">
+        <v>6.6</v>
+      </c>
+      <c r="O77">
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>45615</v>
+        <v>45596</v>
       </c>
       <c r="B78" s="2">
-        <v>178.6</v>
+        <v>179.6</v>
       </c>
       <c r="C78" s="2">
         <v>24.8</v>
       </c>
       <c r="D78" s="3">
-        <v>1059</v>
+        <v>932</v>
       </c>
       <c r="E78" s="3">
-        <v>405</v>
-      </c>
-      <c r="I78" s="3">
-        <v>222</v>
+        <v>352</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="L78">
+        <v>117</v>
       </c>
       <c r="M78" s="3">
-        <v>14195</v>
-      </c>
-      <c r="N78" s="3">
-        <v>5.93</v>
-      </c>
-      <c r="O78" s="3">
-        <v>9</v>
+        <v>13725</v>
+      </c>
+      <c r="N78">
+        <v>5.47</v>
+      </c>
+      <c r="O78">
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>45616</v>
+        <v>45597</v>
       </c>
       <c r="B79" s="2">
-        <v>177.8</v>
+        <v>180</v>
       </c>
       <c r="C79" s="2">
-        <v>24.7</v>
+        <v>24.8</v>
       </c>
       <c r="D79" s="3">
-        <v>1140</v>
-      </c>
-      <c r="G79" s="3">
-        <v>506</v>
+        <v>930</v>
+      </c>
+      <c r="E79" s="3">
+        <v>404</v>
       </c>
       <c r="I79" s="3">
-        <v>252</v>
+        <v>86</v>
       </c>
       <c r="M79" s="3">
-        <v>13323</v>
-      </c>
-      <c r="N79" s="3">
-        <v>5.57</v>
-      </c>
-      <c r="O79" s="3">
-        <v>7</v>
+        <v>10506</v>
+      </c>
+      <c r="N79">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="O79">
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>45617</v>
+        <v>45598</v>
       </c>
       <c r="B80" s="2">
-        <v>178</v>
+        <v>181.3</v>
       </c>
       <c r="C80" s="2">
-        <v>24.7</v>
+        <v>25</v>
       </c>
       <c r="D80" s="3">
-        <v>978</v>
-      </c>
-      <c r="E80" s="3">
-        <v>432</v>
+        <v>860</v>
+      </c>
+      <c r="E80" s="3"/>
+      <c r="F80" s="5">
+        <v>183</v>
       </c>
       <c r="I80" s="3">
-        <v>207</v>
+        <v>350</v>
       </c>
       <c r="M80" s="3">
-        <v>15534</v>
-      </c>
-      <c r="N80" s="3">
-        <v>6.17</v>
-      </c>
-      <c r="O80" s="3">
-        <v>3</v>
+        <v>16473</v>
+      </c>
+      <c r="N80">
+        <v>6.84</v>
+      </c>
+      <c r="O80">
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>45618</v>
+        <v>45599</v>
       </c>
       <c r="B81" s="2">
-        <v>177.8</v>
+        <v>182</v>
       </c>
       <c r="C81" s="2">
-        <v>24.5</v>
+        <v>25.1</v>
       </c>
       <c r="D81" s="3">
-        <v>1038</v>
-      </c>
-      <c r="F81" s="7">
-        <v>312</v>
-      </c>
-      <c r="I81" s="3">
-        <v>330</v>
-      </c>
+        <v>943</v>
+      </c>
+      <c r="E81" s="3">
+        <v>454</v>
+      </c>
+      <c r="I81" s="3"/>
       <c r="M81" s="3">
-        <v>17835</v>
-      </c>
-      <c r="N81" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="O81" s="3">
-        <v>9</v>
+        <v>12084</v>
+      </c>
+      <c r="N81">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="O81">
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>45619</v>
+        <v>45600</v>
       </c>
       <c r="B82" s="2">
-        <v>176.8</v>
+        <v>179.2</v>
       </c>
       <c r="C82" s="2">
-        <v>24.4</v>
+        <v>24.8</v>
       </c>
       <c r="D82" s="3">
-        <v>1122</v>
+        <v>814</v>
       </c>
       <c r="E82" s="3">
-        <v>462</v>
-      </c>
-      <c r="I82" s="3">
-        <v>285</v>
-      </c>
-      <c r="J82" s="3"/>
+        <v>401</v>
+      </c>
       <c r="M82" s="3">
-        <v>14394</v>
-      </c>
-      <c r="N82" s="3">
-        <v>6.21</v>
-      </c>
-      <c r="O82" s="3">
-        <v>4</v>
+        <v>9071</v>
+      </c>
+      <c r="N82">
+        <v>3.57</v>
+      </c>
+      <c r="O82">
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>45620</v>
+        <v>45601</v>
       </c>
       <c r="B83" s="2">
-        <v>177.6</v>
+        <v>180.2</v>
       </c>
       <c r="C83" s="2">
-        <v>24.5</v>
+        <v>24.9</v>
       </c>
       <c r="D83" s="3">
-        <v>1013</v>
-      </c>
-      <c r="G83" s="3">
-        <v>454</v>
-      </c>
-      <c r="I83" s="3">
-        <v>109</v>
-      </c>
-      <c r="J83" s="3"/>
-      <c r="L83" s="3">
-        <v>52</v>
+        <v>648</v>
+      </c>
+      <c r="F83" s="7">
+        <v>174</v>
       </c>
       <c r="M83" s="3">
-        <v>12001</v>
-      </c>
-      <c r="N83" s="3">
-        <v>4.8099999999999996</v>
-      </c>
-      <c r="O83" s="3">
-        <v>9</v>
+        <v>11332</v>
+      </c>
+      <c r="N83">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="O83">
+        <v>2</v>
       </c>
     </row>
     <row r="84" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>45621</v>
+        <v>45602</v>
       </c>
       <c r="B84" s="2">
-        <v>179</v>
+        <v>180.2</v>
       </c>
       <c r="C84" s="2">
-        <v>24.7</v>
+        <v>25.1</v>
       </c>
       <c r="D84" s="3">
-        <v>1092</v>
+        <v>995</v>
       </c>
       <c r="E84" s="3">
-        <v>448</v>
-      </c>
-      <c r="I84" s="3">
-        <v>133</v>
-      </c>
-      <c r="J84" s="3"/>
+        <v>366</v>
+      </c>
       <c r="M84" s="3">
-        <v>14848</v>
-      </c>
-      <c r="N84" s="3">
-        <v>6.14</v>
-      </c>
-      <c r="O84" s="3">
-        <v>14</v>
+        <v>12109</v>
+      </c>
+      <c r="N84">
+        <v>4.8600000000000003</v>
+      </c>
+      <c r="O84">
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>45622</v>
+        <v>45603</v>
       </c>
       <c r="B85" s="2">
-        <v>177.7</v>
+        <v>179.7</v>
       </c>
       <c r="C85" s="2">
-        <v>24.6</v>
+        <v>24.9</v>
       </c>
       <c r="D85" s="3">
-        <v>1049</v>
+        <v>915</v>
       </c>
       <c r="E85" s="3">
-        <v>429</v>
-      </c>
-      <c r="I85" s="3">
-        <v>290</v>
-      </c>
-      <c r="J85" s="3"/>
+        <v>384</v>
+      </c>
       <c r="M85" s="3">
-        <v>15820</v>
-      </c>
-      <c r="N85" s="3">
-        <v>6.63</v>
-      </c>
-      <c r="O85" s="3">
-        <v>9</v>
+        <v>12560</v>
+      </c>
+      <c r="N85">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="O85">
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>45623</v>
-      </c>
-      <c r="B86" s="2">
-        <v>178.4</v>
-      </c>
-      <c r="C86" s="2">
-        <v>24.6</v>
-      </c>
+        <v>45605</v>
+      </c>
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
       <c r="D86" s="3">
-        <v>1097</v>
-      </c>
-      <c r="G86" s="3">
-        <v>454</v>
+        <v>1089</v>
       </c>
       <c r="I86" s="3">
-        <v>65</v>
-      </c>
-      <c r="J86" s="3"/>
+        <v>297</v>
+      </c>
       <c r="M86" s="3">
-        <v>12467</v>
-      </c>
-      <c r="N86" s="3">
-        <v>5.08</v>
-      </c>
-      <c r="O86" s="3">
-        <v>21</v>
+        <v>22554</v>
+      </c>
+      <c r="N86">
+        <v>8.86</v>
+      </c>
+      <c r="O86">
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>45624</v>
-      </c>
-      <c r="B87" s="2">
-        <v>178.7</v>
-      </c>
-      <c r="C87" s="2">
-        <v>24.6</v>
-      </c>
+        <v>45606</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
       <c r="D87" s="3">
-        <v>1211</v>
+        <v>1032</v>
       </c>
       <c r="E87" s="3">
-        <v>424</v>
-      </c>
-      <c r="J87" s="3">
-        <v>193</v>
+        <v>219</v>
+      </c>
+      <c r="I87" s="3">
+        <v>88</v>
       </c>
       <c r="M87" s="3">
-        <v>16809</v>
+        <v>16999</v>
       </c>
       <c r="N87" s="3">
-        <v>7.15</v>
+        <v>6.88</v>
       </c>
       <c r="O87" s="3">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>45625</v>
-      </c>
-      <c r="B88" s="2">
-        <v>177.6</v>
-      </c>
-      <c r="C88" s="2">
-        <v>24.5</v>
-      </c>
+        <v>45607</v>
+      </c>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
       <c r="D88" s="3">
-        <v>1229</v>
-      </c>
-      <c r="E88" s="3">
-        <v>500</v>
-      </c>
-      <c r="J88">
-        <v>262</v>
+        <v>1221</v>
+      </c>
+      <c r="F88" s="7">
+        <v>291</v>
+      </c>
+      <c r="L88" s="3">
+        <v>276</v>
       </c>
       <c r="M88" s="3">
-        <v>18166</v>
+        <v>15849</v>
       </c>
       <c r="N88" s="3">
-        <v>7.62</v>
+        <v>6.55</v>
       </c>
       <c r="O88" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>45626</v>
-      </c>
-      <c r="B89" s="2">
-        <v>177.6</v>
-      </c>
-      <c r="C89" s="2">
-        <v>24.6</v>
-      </c>
+        <v>45608</v>
+      </c>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
       <c r="D89" s="3">
-        <v>1058</v>
-      </c>
-      <c r="G89">
-        <v>457</v>
-      </c>
-      <c r="I89">
-        <v>189</v>
+        <v>1147</v>
+      </c>
+      <c r="F89" s="7">
+        <v>193</v>
+      </c>
+      <c r="I89" s="3">
+        <v>131</v>
+      </c>
+      <c r="L89" s="3">
+        <v>218</v>
       </c>
       <c r="M89" s="3">
-        <v>9577</v>
+        <v>16653</v>
       </c>
       <c r="N89" s="3">
-        <v>3.93</v>
+        <v>6.74</v>
       </c>
       <c r="O89" s="3">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>45627</v>
-      </c>
-      <c r="B90" s="2">
-        <v>178.8</v>
-      </c>
-      <c r="C90" s="2">
-        <v>24.7</v>
-      </c>
+        <v>45609</v>
+      </c>
+      <c r="B90" s="2"/>
+      <c r="C90" s="2"/>
       <c r="D90" s="3">
-        <v>1026</v>
-      </c>
-      <c r="E90">
-        <v>425</v>
-      </c>
-      <c r="I90">
-        <v>295</v>
+        <v>1251</v>
+      </c>
+      <c r="F90" s="7">
+        <v>153</v>
+      </c>
+      <c r="I90" s="3">
+        <v>121</v>
+      </c>
+      <c r="L90" s="3">
+        <v>338</v>
       </c>
       <c r="M90" s="3">
-        <v>15906</v>
+        <v>16897</v>
       </c>
       <c r="N90" s="3">
-        <v>6.49</v>
+        <v>6.66</v>
       </c>
       <c r="O90" s="3">
-        <v>5</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>45628</v>
-      </c>
-      <c r="B91" s="2">
-        <v>179</v>
-      </c>
-      <c r="C91" s="2">
-        <v>24.6</v>
-      </c>
+        <v>45610</v>
+      </c>
+      <c r="B91" s="2"/>
+      <c r="C91" s="2"/>
       <c r="D91" s="3">
-        <v>1182</v>
-      </c>
-      <c r="E91">
-        <v>418</v>
-      </c>
-      <c r="I91">
-        <v>192</v>
+        <v>1033</v>
+      </c>
+      <c r="E91" s="3">
+        <v>250</v>
+      </c>
+      <c r="H91" s="3">
+        <v>118</v>
       </c>
       <c r="M91" s="3">
-        <v>16564</v>
+        <v>14462</v>
       </c>
       <c r="N91" s="3">
-        <v>6.88</v>
+        <v>6.03</v>
       </c>
       <c r="O91" s="3">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>45629</v>
-      </c>
-      <c r="B92" s="2">
-        <v>177.8</v>
-      </c>
-      <c r="C92" s="2">
-        <v>24.6</v>
-      </c>
+        <v>45611</v>
+      </c>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
       <c r="D92" s="3">
-        <v>1068</v>
-      </c>
-      <c r="E92">
-        <v>394</v>
+        <v>882</v>
+      </c>
+      <c r="G92" s="3">
+        <v>227</v>
+      </c>
+      <c r="I92" s="3">
+        <v>36</v>
       </c>
       <c r="M92" s="3">
-        <v>14689</v>
+        <v>12611</v>
       </c>
       <c r="N92" s="3">
-        <v>6.06</v>
+        <v>5.75</v>
       </c>
       <c r="O92" s="3">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>45630</v>
+        <v>45613</v>
       </c>
       <c r="B93" s="2">
-        <v>178</v>
+        <v>180.6</v>
       </c>
       <c r="C93" s="2">
-        <v>24.6</v>
+        <v>24.8</v>
       </c>
       <c r="D93" s="3">
-        <v>964</v>
-      </c>
-      <c r="E93">
-        <v>450</v>
-      </c>
-      <c r="I93">
-        <v>62</v>
+        <v>1146</v>
+      </c>
+      <c r="E93" s="3">
+        <v>439</v>
+      </c>
+      <c r="I93" s="3">
+        <v>207</v>
       </c>
       <c r="M93" s="3">
-        <v>7608</v>
+        <v>16282</v>
       </c>
       <c r="N93" s="3">
-        <v>3.05</v>
+        <v>6.94</v>
       </c>
       <c r="O93" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>45631</v>
+        <v>45614</v>
       </c>
       <c r="B94" s="2">
-        <v>178.5</v>
+        <v>179.6</v>
       </c>
       <c r="C94" s="2">
-        <v>24.7</v>
+        <v>24.9</v>
       </c>
       <c r="D94" s="3">
-        <v>1016</v>
-      </c>
-      <c r="E94">
-        <v>403</v>
-      </c>
-      <c r="I94">
-        <v>255</v>
+        <v>1057</v>
+      </c>
+      <c r="E94" s="3">
+        <v>420</v>
+      </c>
+      <c r="I94" s="3">
+        <v>158</v>
       </c>
       <c r="M94" s="3">
-        <v>14538</v>
+        <v>15864</v>
       </c>
       <c r="N94" s="3">
-        <v>5.91</v>
+        <v>6.53</v>
       </c>
       <c r="O94" s="3">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>45632</v>
+        <v>45615</v>
       </c>
       <c r="B95" s="2">
-        <v>178.7</v>
+        <v>178.6</v>
       </c>
       <c r="C95" s="2">
-        <v>24.7</v>
+        <v>24.8</v>
       </c>
       <c r="D95" s="3">
-        <v>981</v>
-      </c>
-      <c r="E95">
-        <v>446</v>
-      </c>
-      <c r="I95">
-        <v>137</v>
+        <v>1059</v>
+      </c>
+      <c r="E95" s="3">
+        <v>405</v>
+      </c>
+      <c r="I95" s="3">
+        <v>222</v>
       </c>
       <c r="M95" s="3">
-        <v>12493</v>
+        <v>14195</v>
       </c>
       <c r="N95" s="3">
-        <v>4.96</v>
+        <v>5.93</v>
       </c>
       <c r="O95" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
+        <v>45616</v>
+      </c>
+      <c r="B96" s="2">
+        <v>177.8</v>
+      </c>
+      <c r="C96" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="D96" s="3">
+        <v>1140</v>
+      </c>
+      <c r="G96" s="3">
+        <v>506</v>
+      </c>
+      <c r="I96" s="3">
+        <v>252</v>
+      </c>
+      <c r="M96" s="3">
+        <v>13323</v>
+      </c>
+      <c r="N96" s="3">
+        <v>5.57</v>
+      </c>
+      <c r="O96" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>45617</v>
+      </c>
+      <c r="B97" s="2">
+        <v>178</v>
+      </c>
+      <c r="C97" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="D97" s="3">
+        <v>978</v>
+      </c>
+      <c r="E97" s="3">
+        <v>432</v>
+      </c>
+      <c r="I97" s="3">
+        <v>207</v>
+      </c>
+      <c r="M97" s="3">
+        <v>15534</v>
+      </c>
+      <c r="N97" s="3">
+        <v>6.17</v>
+      </c>
+      <c r="O97" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>45618</v>
+      </c>
+      <c r="B98" s="2">
+        <v>177.8</v>
+      </c>
+      <c r="C98" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="D98" s="3">
+        <v>1038</v>
+      </c>
+      <c r="F98" s="7">
+        <v>312</v>
+      </c>
+      <c r="I98" s="3">
+        <v>330</v>
+      </c>
+      <c r="M98" s="3">
+        <v>17835</v>
+      </c>
+      <c r="N98" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="O98" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>45619</v>
+      </c>
+      <c r="B99" s="2">
+        <v>176.8</v>
+      </c>
+      <c r="C99" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="D99" s="3">
+        <v>1122</v>
+      </c>
+      <c r="E99" s="3">
+        <v>462</v>
+      </c>
+      <c r="I99" s="3">
+        <v>285</v>
+      </c>
+      <c r="J99" s="3"/>
+      <c r="M99" s="3">
+        <v>14394</v>
+      </c>
+      <c r="N99" s="3">
+        <v>6.21</v>
+      </c>
+      <c r="O99" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>45620</v>
+      </c>
+      <c r="B100" s="2">
+        <v>177.6</v>
+      </c>
+      <c r="C100" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="D100" s="3">
+        <v>1013</v>
+      </c>
+      <c r="G100" s="3">
+        <v>454</v>
+      </c>
+      <c r="I100" s="3">
+        <v>109</v>
+      </c>
+      <c r="J100" s="3"/>
+      <c r="L100" s="3">
+        <v>52</v>
+      </c>
+      <c r="M100" s="3">
+        <v>12001</v>
+      </c>
+      <c r="N100" s="3">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="O100" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>45621</v>
+      </c>
+      <c r="B101" s="2">
+        <v>179</v>
+      </c>
+      <c r="C101" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="D101" s="3">
+        <v>1092</v>
+      </c>
+      <c r="E101" s="3">
+        <v>448</v>
+      </c>
+      <c r="I101" s="3">
+        <v>133</v>
+      </c>
+      <c r="J101" s="3"/>
+      <c r="M101" s="3">
+        <v>14848</v>
+      </c>
+      <c r="N101" s="3">
+        <v>6.14</v>
+      </c>
+      <c r="O101" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>45622</v>
+      </c>
+      <c r="B102" s="2">
+        <v>177.7</v>
+      </c>
+      <c r="C102" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="D102" s="3">
+        <v>1049</v>
+      </c>
+      <c r="E102" s="3">
+        <v>429</v>
+      </c>
+      <c r="I102" s="3">
+        <v>290</v>
+      </c>
+      <c r="J102" s="3"/>
+      <c r="M102" s="3">
+        <v>15820</v>
+      </c>
+      <c r="N102" s="3">
+        <v>6.63</v>
+      </c>
+      <c r="O102" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>45623</v>
+      </c>
+      <c r="B103" s="2">
+        <v>178.4</v>
+      </c>
+      <c r="C103" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="D103" s="3">
+        <v>1097</v>
+      </c>
+      <c r="G103" s="3">
+        <v>454</v>
+      </c>
+      <c r="I103" s="3">
+        <v>65</v>
+      </c>
+      <c r="J103" s="3"/>
+      <c r="M103" s="3">
+        <v>12467</v>
+      </c>
+      <c r="N103" s="3">
+        <v>5.08</v>
+      </c>
+      <c r="O103" s="3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>45624</v>
+      </c>
+      <c r="B104" s="2">
+        <v>178.7</v>
+      </c>
+      <c r="C104" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="D104" s="3">
+        <v>1211</v>
+      </c>
+      <c r="E104" s="3">
+        <v>424</v>
+      </c>
+      <c r="J104" s="3">
+        <v>193</v>
+      </c>
+      <c r="M104" s="3">
+        <v>16809</v>
+      </c>
+      <c r="N104" s="3">
+        <v>7.15</v>
+      </c>
+      <c r="O104" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>45625</v>
+      </c>
+      <c r="B105" s="2">
+        <v>177.6</v>
+      </c>
+      <c r="C105" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="D105" s="3">
+        <v>1229</v>
+      </c>
+      <c r="E105" s="3">
+        <v>500</v>
+      </c>
+      <c r="J105">
+        <v>262</v>
+      </c>
+      <c r="M105" s="3">
+        <v>18166</v>
+      </c>
+      <c r="N105" s="3">
+        <v>7.62</v>
+      </c>
+      <c r="O105" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>45626</v>
+      </c>
+      <c r="B106" s="2">
+        <v>177.6</v>
+      </c>
+      <c r="C106" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="D106" s="3">
+        <v>1058</v>
+      </c>
+      <c r="G106">
+        <v>457</v>
+      </c>
+      <c r="I106">
+        <v>189</v>
+      </c>
+      <c r="M106" s="3">
+        <v>9577</v>
+      </c>
+      <c r="N106" s="3">
+        <v>3.93</v>
+      </c>
+      <c r="O106" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>45627</v>
+      </c>
+      <c r="B107" s="2">
+        <v>178.8</v>
+      </c>
+      <c r="C107" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="D107" s="3">
+        <v>1026</v>
+      </c>
+      <c r="E107">
+        <v>425</v>
+      </c>
+      <c r="I107">
+        <v>295</v>
+      </c>
+      <c r="M107" s="3">
+        <v>15906</v>
+      </c>
+      <c r="N107" s="3">
+        <v>6.49</v>
+      </c>
+      <c r="O107" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>45628</v>
+      </c>
+      <c r="B108" s="2">
+        <v>179</v>
+      </c>
+      <c r="C108" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="D108" s="3">
+        <v>1182</v>
+      </c>
+      <c r="E108">
+        <v>418</v>
+      </c>
+      <c r="I108">
+        <v>192</v>
+      </c>
+      <c r="M108" s="3">
+        <v>16564</v>
+      </c>
+      <c r="N108" s="3">
+        <v>6.88</v>
+      </c>
+      <c r="O108" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>45629</v>
+      </c>
+      <c r="B109" s="2">
+        <v>177.8</v>
+      </c>
+      <c r="C109" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="D109" s="3">
+        <v>1068</v>
+      </c>
+      <c r="E109">
+        <v>394</v>
+      </c>
+      <c r="M109" s="3">
+        <v>14689</v>
+      </c>
+      <c r="N109" s="3">
+        <v>6.06</v>
+      </c>
+      <c r="O109" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>45630</v>
+      </c>
+      <c r="B110" s="2">
+        <v>178</v>
+      </c>
+      <c r="C110" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="D110" s="3">
+        <v>964</v>
+      </c>
+      <c r="E110">
+        <v>450</v>
+      </c>
+      <c r="I110">
+        <v>62</v>
+      </c>
+      <c r="M110" s="3">
+        <v>7608</v>
+      </c>
+      <c r="N110" s="3">
+        <v>3.05</v>
+      </c>
+      <c r="O110" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>45631</v>
+      </c>
+      <c r="B111" s="2">
+        <v>178.5</v>
+      </c>
+      <c r="C111" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="D111" s="3">
+        <v>1016</v>
+      </c>
+      <c r="E111">
+        <v>403</v>
+      </c>
+      <c r="I111">
+        <v>255</v>
+      </c>
+      <c r="M111" s="3">
+        <v>14538</v>
+      </c>
+      <c r="N111" s="3">
+        <v>5.91</v>
+      </c>
+      <c r="O111" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>45632</v>
+      </c>
+      <c r="B112" s="2">
+        <v>178.7</v>
+      </c>
+      <c r="C112" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="D112" s="3">
+        <v>981</v>
+      </c>
+      <c r="E112">
+        <v>446</v>
+      </c>
+      <c r="I112">
+        <v>137</v>
+      </c>
+      <c r="M112" s="3">
+        <v>12493</v>
+      </c>
+      <c r="N112" s="3">
+        <v>4.96</v>
+      </c>
+      <c r="O112" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
         <v>45633</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B113" s="2">
         <v>177.4</v>
       </c>
-      <c r="C96" s="2">
+      <c r="C113" s="2">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="1"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-    </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="1"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-    </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="1"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-    </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="1"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-    </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="1"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-    </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="1"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-    </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="1"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-    </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="1"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-    </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="1"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-    </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="1"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-    </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="1"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="1"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-    </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="1"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-    </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="1"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="1"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="1"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-    </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="1"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-    </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="1"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-    </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D113">
+        <v>1118</v>
+      </c>
+      <c r="F113" s="5">
+        <v>327</v>
+      </c>
+      <c r="I113">
+        <v>271</v>
+      </c>
+      <c r="M113">
+        <v>18127</v>
+      </c>
+      <c r="N113">
+        <v>7.63</v>
+      </c>
+      <c r="O113" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>45634</v>
+      </c>
+      <c r="B114" s="2">
+        <v>178.8</v>
+      </c>
+      <c r="C114" s="2">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -7270,6 +7644,91 @@
       <c r="A1014" s="1"/>
       <c r="B1014" s="2"/>
       <c r="C1014" s="2"/>
+    </row>
+    <row r="1015" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1015" s="1"/>
+      <c r="B1015" s="2"/>
+      <c r="C1015" s="2"/>
+    </row>
+    <row r="1016" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1016" s="1"/>
+      <c r="B1016" s="2"/>
+      <c r="C1016" s="2"/>
+    </row>
+    <row r="1017" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1017" s="1"/>
+      <c r="B1017" s="2"/>
+      <c r="C1017" s="2"/>
+    </row>
+    <row r="1018" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1018" s="1"/>
+      <c r="B1018" s="2"/>
+      <c r="C1018" s="2"/>
+    </row>
+    <row r="1019" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1019" s="1"/>
+      <c r="B1019" s="2"/>
+      <c r="C1019" s="2"/>
+    </row>
+    <row r="1020" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1020" s="1"/>
+      <c r="B1020" s="2"/>
+      <c r="C1020" s="2"/>
+    </row>
+    <row r="1021" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1021" s="1"/>
+      <c r="B1021" s="2"/>
+      <c r="C1021" s="2"/>
+    </row>
+    <row r="1022" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="2"/>
+      <c r="C1022" s="2"/>
+    </row>
+    <row r="1023" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="2"/>
+      <c r="C1023" s="2"/>
+    </row>
+    <row r="1024" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="2"/>
+      <c r="C1024" s="2"/>
+    </row>
+    <row r="1025" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="2"/>
+      <c r="C1025" s="2"/>
+    </row>
+    <row r="1026" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1026" s="1"/>
+      <c r="B1026" s="2"/>
+      <c r="C1026" s="2"/>
+    </row>
+    <row r="1027" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1027" s="1"/>
+      <c r="B1027" s="2"/>
+      <c r="C1027" s="2"/>
+    </row>
+    <row r="1028" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1028" s="1"/>
+      <c r="B1028" s="2"/>
+      <c r="C1028" s="2"/>
+    </row>
+    <row r="1029" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1029" s="1"/>
+      <c r="B1029" s="2"/>
+      <c r="C1029" s="2"/>
+    </row>
+    <row r="1030" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1030" s="1"/>
+      <c r="B1030" s="2"/>
+      <c r="C1030" s="2"/>
+    </row>
+    <row r="1031" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1031" s="1"/>
+      <c r="B1031" s="2"/>
+      <c r="C1031" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -7285,7 +7744,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
data entry and cosmetic
</commit_message>
<xml_diff>
--- a/book_data/Fitness.xlsx
+++ b/book_data/Fitness.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edmundlskoviak/Library/Mobile Documents/com~apple~CloudDocs/Data Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D8AE84-D326-C445-A7E4-CD9BA408F077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DEAA70-EAFA-694A-9AC7-F61BC47FF928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2960" yWindow="2260" windowWidth="28200" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,9 @@
   <si>
     <t>dist</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -157,6 +160,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,7 +382,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B103" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E116" sqref="E116"/>
+      <selection pane="bottomRight" activeCell="J117" sqref="J117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3190,16 +3194,61 @@
       <c r="C116" s="2">
         <v>24.7</v>
       </c>
+      <c r="D116">
+        <v>1094</v>
+      </c>
+      <c r="E116">
+        <v>410</v>
+      </c>
+      <c r="M116">
+        <v>15259</v>
+      </c>
+      <c r="N116">
+        <v>6.28</v>
+      </c>
+      <c r="O116" s="3">
+        <v>14</v>
+      </c>
     </row>
     <row r="117" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="1"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
+      <c r="A117" s="1">
+        <v>45637</v>
+      </c>
+      <c r="B117" s="2">
+        <v>178.6</v>
+      </c>
+      <c r="C117" s="2">
+        <v>24.5</v>
+      </c>
+      <c r="D117">
+        <v>1097</v>
+      </c>
+      <c r="G117">
+        <v>393</v>
+      </c>
+      <c r="I117">
+        <v>278</v>
+      </c>
+      <c r="M117">
+        <v>13578</v>
+      </c>
+      <c r="N117">
+        <v>5.78</v>
+      </c>
+      <c r="O117" s="3">
+        <v>12</v>
+      </c>
     </row>
     <row r="118" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="1"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
+      <c r="A118" s="1">
+        <v>45638</v>
+      </c>
+      <c r="B118" s="2">
+        <v>181.2</v>
+      </c>
+      <c r="C118" s="2">
+        <v>25</v>
+      </c>
     </row>
     <row r="119" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
@@ -7774,10 +7823,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D72D56F-EAA6-F445-AD3E-C9C4047DF54B}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7905,6 +7954,43 @@
         <v>0.69239766081871346</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>45636</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>1171</v>
+      </c>
+      <c r="E7">
+        <v>0.46</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>45636</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>223</v>
+      </c>
+      <c r="D8">
+        <v>5766</v>
+      </c>
+      <c r="E8">
+        <v>2.5099999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>